<commit_message>
Training Plan - Update
</commit_message>
<xml_diff>
--- a/Project List.xlsx
+++ b/Project List.xlsx
@@ -214,17 +214,17 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.5663265306123"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="44.6836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.8928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="44.1428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Project List - Update
</commit_message>
<xml_diff>
--- a/Project List.xlsx
+++ b/Project List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t xml:space="preserve">Project Name</t>
   </si>
@@ -83,6 +83,54 @@
   </si>
   <si>
     <t xml:space="preserve">It is a donation app, which will make the excess stuff of anyone used by someone needy. Its like OLX.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Police Alert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umair, Saad Ahmed, Muhammad Ata Jilani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Police Alert Mobile Application enables citizens of the Karachi Police to receive various Safety, Security and Public services. You can avail various Police services through mobile phone. The efforts to improvise and add new services will continue. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joystick Application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umair Shuja, Sarang, Zohaib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appoint A Doctor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android studio,java,xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atoofa Akber, Hafiz Umer Bin Nasir, Soha Gazdar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This app alllows user to find Doctors in Karachi and appoint them by Call(if this service provided by them) and also this app allow user to interact with emergency services in case of Emergency.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android Voting System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android Studio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junaid Shabbir, Muhammad Ghazali, Hamza Khalid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This application provides is a new technique of casting votes using mobile phones. Android voting system is an application developed for android devices to deploy an easy and flexible way of casting votes anytime and from anywhere.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shop in budget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android, JSON, PHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jawahir Qayyum</t>
   </si>
 </sst>
 </file>
@@ -92,7 +140,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -123,6 +171,13 @@
     <font>
       <b val="true"/>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -170,7 +225,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -193,6 +248,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -212,19 +271,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.8928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="44.1428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="62.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.8724489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="43.0612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -255,7 +314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="128.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="141.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -307,6 +366,70 @@
       </c>
       <c r="D6" s="5" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="90.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="65.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="77.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>